<commit_message>
add blank schedule template excel spreadsheet
</commit_message>
<xml_diff>
--- a/schedule-template/Template-schedule-blank.xlsx
+++ b/schedule-template/Template-schedule-blank.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10404"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dannykaiwatson/Documents/coding/git repos/work-experience-at-ncl-uni-rse-dept/schedule-template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF06A012-EE3E-6A4A-975B-A872D904ABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{FF06A012-EE3E-6A4A-975B-A872D904ABBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61A8A358-B0A8-0B48-9767-43DCF345A681}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{C650EF95-26C9-584A-98DD-0A0EFCC8CB4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="5">
   <si>
     <t>From</t>
   </si>
@@ -46,9 +47,6 @@
   </si>
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>q</t>
   </si>
 </sst>
 </file>
@@ -404,10 +402,10 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="A2:D5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -441,9 +439,7 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="D5" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>